<commit_message>
update laporan pagination and fix register siswa excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userr\Desktop\project absenmaganh\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE45AE06-4B30-4B0D-9C2F-D793114E9400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B590567C-E430-4827-8B2D-D7DF072391EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03518207-9859-4204-9B6A-CC02AB3D88DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -33,41 +33,35 @@
     <t>username</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>namaJurusan</t>
   </si>
   <si>
-    <t>siswa</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>testsuswa</t>
-  </si>
-  <si>
-    <t>testadmin</t>
-  </si>
-  <si>
-    <t>testsiswa</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>X AKL1</t>
+  </si>
+  <si>
+    <t>testsiswanew</t>
+  </si>
+  <si>
+    <t>testadminnew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDDD04D-A769-46D8-9099-00F59110FA69}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,7 +415,7 @@
     <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,36 +425,31 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>